<commit_message>
moved F82H handbook notes to the F82H folder
</commit_message>
<xml_diff>
--- a/Jupyter/OutputFeatures.xlsx
+++ b/Jupyter/OutputFeatures.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuqih\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Repos\DatabaseCodes\Jupyter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2154355A-5BF2-432E-943A-435356C08A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8478CE9B-8909-481E-9561-665810EB7D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="68">
   <si>
     <t>Target1</t>
   </si>
@@ -126,15 +126,9 @@
     <t>bar/plate</t>
   </si>
   <si>
-    <t>Grain Size</t>
-  </si>
-  <si>
     <t>dpa</t>
   </si>
   <si>
-    <t>he</t>
-  </si>
-  <si>
     <t>Austenizing time</t>
   </si>
   <si>
@@ -144,18 +138,12 @@
     <t>Size</t>
   </si>
   <si>
-    <t>Austenizing temp</t>
-  </si>
-  <si>
     <t>Tempering temp</t>
   </si>
   <si>
     <t>aged temp</t>
   </si>
   <si>
-    <t>aged time</t>
-  </si>
-  <si>
     <t>Feature14</t>
   </si>
   <si>
@@ -220,6 +208,27 @@
   </si>
   <si>
     <t>EUROFER97, aged 700 °C 12000 h, transverse</t>
+  </si>
+  <si>
+    <t>aged time (hr)</t>
+  </si>
+  <si>
+    <t>Feature15</t>
+  </si>
+  <si>
+    <t>polished</t>
+  </si>
+  <si>
+    <t>surface finish</t>
+  </si>
+  <si>
+    <t>Grain Size (micron)</t>
+  </si>
+  <si>
+    <t>He (appm)</t>
+  </si>
+  <si>
+    <t>Austenizing temp (C)</t>
   </si>
 </sst>
 </file>
@@ -303,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -342,6 +351,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -624,33 +639,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S148"/>
+  <dimension ref="A1:T148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="65.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="65.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" style="2" customWidth="1"/>
     <col min="3" max="5" width="6" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" style="2" customWidth="1"/>
     <col min="8" max="8" width="11" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" style="2" customWidth="1"/>
-    <col min="12" max="13" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.453125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="16.54296875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" style="2" customWidth="1"/>
+    <col min="12" max="13" width="8.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18" style="8" customWidth="1"/>
-    <col min="15" max="15" width="17.42578125" style="8" customWidth="1"/>
-    <col min="16" max="16" width="17.85546875" style="8" customWidth="1"/>
-    <col min="17" max="17" width="17.140625" style="8" customWidth="1"/>
-    <col min="18" max="19" width="13.140625" style="8" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="1"/>
+    <col min="15" max="15" width="17.453125" style="8" customWidth="1"/>
+    <col min="16" max="16" width="17.81640625" style="8" customWidth="1"/>
+    <col min="17" max="17" width="17.1796875" style="8" customWidth="1"/>
+    <col min="18" max="19" width="13.1796875" style="8" customWidth="1"/>
+    <col min="20" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -706,10 +721,13 @@
         <v>18</v>
       </c>
       <c r="S1" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>20</v>
       </c>
@@ -732,40 +750,43 @@
         <v>32</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>41</v>
-      </c>
       <c r="S2" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
@@ -799,7 +820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>19</v>
       </c>
@@ -833,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
@@ -867,7 +888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
@@ -901,7 +922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
@@ -935,7 +956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
@@ -969,7 +990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
@@ -1007,7 +1028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>23</v>
       </c>
@@ -1045,7 +1066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>23</v>
       </c>
@@ -1083,7 +1104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -1121,7 +1142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>23</v>
       </c>
@@ -1159,7 +1180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>24</v>
       </c>
@@ -1193,7 +1214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>24</v>
       </c>
@@ -1227,7 +1248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>24</v>
       </c>
@@ -1261,7 +1282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>24</v>
       </c>
@@ -1295,7 +1316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>24</v>
       </c>
@@ -1332,7 +1353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>25</v>
       </c>
@@ -1373,7 +1394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>25</v>
       </c>
@@ -1414,7 +1435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>25</v>
       </c>
@@ -1455,7 +1476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>25</v>
       </c>
@@ -1496,7 +1517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>25</v>
       </c>
@@ -1537,7 +1558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>26</v>
       </c>
@@ -1578,7 +1599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>26</v>
       </c>
@@ -1619,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>26</v>
       </c>
@@ -1660,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>26</v>
       </c>
@@ -1701,7 +1722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>26</v>
       </c>
@@ -1742,48 +1763,65 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="7">
+    <row r="29" spans="1:20" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="14">
         <v>659.84305406177998</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" s="10">
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" s="14">
         <v>21.033555944724601</v>
       </c>
-      <c r="H29" s="10" t="s">
+      <c r="H29" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I29" s="10">
+      <c r="I29" s="14">
         <v>8</v>
       </c>
-      <c r="J29" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5">
-        <v>0</v>
-      </c>
-      <c r="S29" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J29" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="K29" s="3">
+        <v>7</v>
+      </c>
+      <c r="L29" s="3">
+        <v>0</v>
+      </c>
+      <c r="M29" s="3">
+        <v>0</v>
+      </c>
+      <c r="N29" s="3">
+        <v>1075</v>
+      </c>
+      <c r="O29" s="3">
+        <v>30</v>
+      </c>
+      <c r="P29" s="3">
+        <v>750</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>120</v>
+      </c>
+      <c r="R29" s="3">
+        <v>600</v>
+      </c>
+      <c r="S29" s="3">
+        <v>1000</v>
+      </c>
+      <c r="T29" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B30" s="7">
         <v>581.12589559877097</v>
@@ -1804,7 +1842,7 @@
         <v>8</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
@@ -1820,9 +1858,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B31" s="7">
         <v>507.37631041293503</v>
@@ -1843,7 +1881,7 @@
         <v>8</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
@@ -1859,9 +1897,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B32" s="7">
         <v>429.42339331979201</v>
@@ -1882,7 +1920,7 @@
         <v>8</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
@@ -1898,9 +1936,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B33" s="7">
         <v>663.28215334530103</v>
@@ -1921,7 +1959,7 @@
         <v>14</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
@@ -1937,9 +1975,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B34" s="7">
         <v>650.67212263905697</v>
@@ -1960,7 +1998,7 @@
         <v>14</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
@@ -1976,9 +2014,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B35" s="7">
         <v>516.16512552376503</v>
@@ -1999,7 +2037,7 @@
         <v>14</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
@@ -2015,9 +2053,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B36" s="7">
         <v>498.20537899021201</v>
@@ -2038,7 +2076,7 @@
         <v>14</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
@@ -2054,9 +2092,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B37" s="7">
         <v>466.10711901068299</v>
@@ -2077,7 +2115,7 @@
         <v>14</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
@@ -2093,9 +2131,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B38" s="7">
         <v>417.57760398341497</v>
@@ -2116,7 +2154,7 @@
         <v>14</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
@@ -2132,9 +2170,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B39" s="7">
         <v>395.79664185444898</v>
@@ -2155,7 +2193,7 @@
         <v>14</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
@@ -2171,9 +2209,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B40" s="7">
         <v>367.13748115844101</v>
@@ -2194,7 +2232,7 @@
         <v>14</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
@@ -2210,9 +2248,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A41" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B41" s="7">
         <v>322.81132427672401</v>
@@ -2233,7 +2271,7 @@
         <v>14</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
@@ -2249,9 +2287,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A42" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B42" s="7">
         <v>314.02250916589298</v>
@@ -2272,7 +2310,7 @@
         <v>14</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
@@ -2288,9 +2326,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B43" s="7">
         <v>290.33093049313902</v>
@@ -2311,7 +2349,7 @@
         <v>14</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
@@ -2327,9 +2365,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B44" s="7">
         <v>275.04603312715898</v>
@@ -2350,7 +2388,7 @@
         <v>14</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
@@ -2366,9 +2404,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A45" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B45" s="7">
         <v>233.39474290517799</v>
@@ -2389,7 +2427,7 @@
         <v>14</v>
       </c>
       <c r="J45" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
@@ -2405,9 +2443,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B46" s="7">
         <v>171.87305462152901</v>
@@ -2428,7 +2466,7 @@
         <v>14</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
@@ -2444,9 +2482,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B47" s="7">
         <v>679.331283335065</v>
@@ -2467,7 +2505,7 @@
         <v>25</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
@@ -2483,9 +2521,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A48" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B48" s="7">
         <v>672.45308476802302</v>
@@ -2506,7 +2544,7 @@
         <v>25</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
@@ -2522,9 +2560,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B49" s="7">
         <v>652.582730436764</v>
@@ -2545,7 +2583,7 @@
         <v>25</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
@@ -2561,9 +2599,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B50" s="7">
         <v>648.76151484135096</v>
@@ -2584,7 +2622,7 @@
         <v>25</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
@@ -2600,9 +2638,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B51" s="7">
         <v>565.84099823279098</v>
@@ -2623,7 +2661,7 @@
         <v>25</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
@@ -2639,9 +2677,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B52" s="7">
         <v>574.629813343622</v>
@@ -2662,7 +2700,7 @@
         <v>25</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
@@ -2678,9 +2716,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B53" s="7">
         <v>534.88910468110203</v>
@@ -2701,7 +2739,7 @@
         <v>25</v>
       </c>
       <c r="J53" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
@@ -2717,9 +2755,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B54" s="7">
         <v>554.75946775844398</v>
@@ -2740,7 +2778,7 @@
         <v>25</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
@@ -2756,9 +2794,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B55" s="7">
         <v>506.229943985094</v>
@@ -2779,7 +2817,7 @@
         <v>25</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
@@ -2795,9 +2833,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B56" s="7">
         <v>497.44114636642701</v>
@@ -2818,7 +2856,7 @@
         <v>25</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
@@ -2834,9 +2872,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B57" s="7">
         <v>434.00885903115397</v>
@@ -2857,7 +2895,7 @@
         <v>25</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
@@ -2873,9 +2911,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B58" s="7">
         <v>431.33399237141703</v>
@@ -2896,7 +2934,7 @@
         <v>25</v>
       </c>
       <c r="J58" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
@@ -2912,9 +2950,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B59" s="7">
         <v>404.96756453108998</v>
@@ -2935,7 +2973,7 @@
         <v>25</v>
       </c>
       <c r="J59" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
@@ -2951,9 +2989,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A60" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B60" s="7">
         <v>398.471499768103</v>
@@ -2974,7 +3012,7 @@
         <v>25</v>
       </c>
       <c r="J60" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
@@ -2990,9 +3028,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B61" s="7">
         <v>627.74479408225102</v>
@@ -3013,7 +3051,7 @@
         <v>100</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
@@ -3029,9 +3067,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A62" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B62" s="7">
         <v>592.97167618906701</v>
@@ -3052,7 +3090,7 @@
         <v>100</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
@@ -3068,9 +3106,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B63" s="7">
         <v>589.91469321743796</v>
@@ -3091,7 +3129,7 @@
         <v>100</v>
       </c>
       <c r="J63" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
@@ -3107,9 +3145,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A64" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B64" s="7">
         <v>519.98634111917795</v>
@@ -3130,7 +3168,7 @@
         <v>100</v>
       </c>
       <c r="J64" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
@@ -3146,9 +3184,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A65" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B65" s="7">
         <v>513.87239266808399</v>
@@ -3169,7 +3207,7 @@
         <v>100</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
@@ -3185,9 +3223,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A66" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B66" s="7">
         <v>487.505964827757</v>
@@ -3208,7 +3246,7 @@
         <v>100</v>
       </c>
       <c r="J66" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
@@ -3224,9 +3262,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A67" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B67" s="7">
         <v>445.09038950550098</v>
@@ -3247,7 +3285,7 @@
         <v>100</v>
       </c>
       <c r="J67" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
@@ -3263,9 +3301,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A68" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B68" s="7">
         <v>423.69156118059101</v>
@@ -3286,7 +3324,7 @@
         <v>100</v>
       </c>
       <c r="J68" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
@@ -3302,9 +3340,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A69" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B69" s="7">
         <v>404.20333190730503</v>
@@ -3325,7 +3363,7 @@
         <v>100</v>
       </c>
       <c r="J69" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
@@ -3341,9 +3379,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A70" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B70" s="7">
         <v>291.47730566706099</v>
@@ -3364,7 +3402,7 @@
         <v>100</v>
       </c>
       <c r="J70" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
@@ -3380,9 +3418,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A71" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B71" s="7">
         <v>282.68849055623002</v>
@@ -3403,7 +3441,7 @@
         <v>100</v>
       </c>
       <c r="J71" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
@@ -3419,9 +3457,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A72" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B72" s="7">
         <v>162.31999814083201</v>
@@ -3442,7 +3480,7 @@
         <v>100</v>
       </c>
       <c r="J72" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
@@ -3458,9 +3496,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A73" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B73" s="7">
         <v>514.254517726058</v>
@@ -3481,7 +3519,7 @@
         <v>14</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
@@ -3497,9 +3535,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A74" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B74" s="7">
         <v>472.60320126583201</v>
@@ -3520,7 +3558,7 @@
         <v>14</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
@@ -3536,9 +3574,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A75" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B75" s="7">
         <v>404.585465711361</v>
@@ -3559,7 +3597,7 @@
         <v>14</v>
       </c>
       <c r="J75" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
@@ -3575,9 +3613,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A76" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B76" s="7">
         <v>369.43022276020298</v>
@@ -3598,7 +3636,7 @@
         <v>14</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
@@ -3614,9 +3652,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A77" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B77" s="7">
         <v>268.54995961809101</v>
@@ -3637,7 +3675,7 @@
         <v>14</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
@@ -3653,9 +3691,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A78" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B78" s="7">
         <v>229.191402251791</v>
@@ -3676,7 +3714,7 @@
         <v>14</v>
       </c>
       <c r="J78" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
@@ -3692,9 +3730,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A79" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B79" s="7">
         <v>152.002717782433</v>
@@ -3715,7 +3753,7 @@
         <v>14</v>
       </c>
       <c r="J79" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
@@ -3731,9 +3769,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A80" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B80" s="7">
         <v>658.69668763393997</v>
@@ -3754,7 +3792,7 @@
         <v>25</v>
       </c>
       <c r="J80" s="10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
@@ -3770,9 +3808,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A81" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B81" s="7">
         <v>667.48549399868796</v>
@@ -3793,7 +3831,7 @@
         <v>25</v>
       </c>
       <c r="J81" s="10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
@@ -3809,9 +3847,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A82" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B82" s="7">
         <v>541.38518693625201</v>
@@ -3832,7 +3870,7 @@
         <v>25</v>
       </c>
       <c r="J82" s="10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K82" s="5"/>
       <c r="L82" s="5"/>
@@ -3848,9 +3886,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A83" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B83" s="7">
         <v>551.70248478681503</v>
@@ -3871,7 +3909,7 @@
         <v>25</v>
       </c>
       <c r="J83" s="10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K83" s="5"/>
       <c r="L83" s="5"/>
@@ -3887,9 +3925,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A84" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B84" s="7">
         <v>673.98157625383806</v>
@@ -3910,7 +3948,7 @@
         <v>100</v>
       </c>
       <c r="J84" s="10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="K84" s="5"/>
       <c r="L84" s="5"/>
@@ -3926,9 +3964,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A85" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B85" s="7">
         <v>318.99009993522901</v>
@@ -3949,7 +3987,7 @@
         <v>100</v>
       </c>
       <c r="J85" s="10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="K85" s="5"/>
       <c r="L85" s="5"/>
@@ -3965,9 +4003,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A86" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B86" s="11">
         <v>661.02088371176296</v>
@@ -3984,7 +4022,7 @@
       <c r="H86" s="10"/>
       <c r="I86" s="10"/>
       <c r="J86" s="10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K86" s="5"/>
       <c r="L86" s="5"/>
@@ -4000,9 +4038,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A87" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B87" s="11">
         <v>475.40603362300402</v>
@@ -4019,7 +4057,7 @@
       <c r="H87" s="10"/>
       <c r="I87" s="10"/>
       <c r="J87" s="10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K87" s="5"/>
       <c r="L87" s="5"/>
@@ -4035,9 +4073,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A88" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B88" s="11">
         <v>405.33643570677401</v>
@@ -4054,7 +4092,7 @@
       <c r="H88" s="10"/>
       <c r="I88" s="10"/>
       <c r="J88" s="10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K88" s="5"/>
       <c r="L88" s="5"/>
@@ -4070,9 +4108,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A89" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B89" s="11">
         <v>271.69374066899701</v>
@@ -4089,7 +4127,7 @@
       <c r="H89" s="10"/>
       <c r="I89" s="10"/>
       <c r="J89" s="10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K89" s="5"/>
       <c r="L89" s="5"/>
@@ -4105,9 +4143,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A90" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B90" s="11">
         <v>154.75639180428701</v>
@@ -4124,7 +4162,7 @@
       <c r="H90" s="10"/>
       <c r="I90" s="10"/>
       <c r="J90" s="10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K90" s="5"/>
       <c r="L90" s="5"/>
@@ -4140,9 +4178,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B91" s="7">
         <v>666</v>
@@ -4176,9 +4214,9 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A92" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B92" s="7">
         <v>537</v>
@@ -4212,9 +4250,9 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A93" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B93" s="7">
         <v>503</v>
@@ -4248,9 +4286,9 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A94" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B94" s="7">
         <v>422</v>
@@ -4284,9 +4322,9 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A95" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B95" s="7">
         <v>296</v>
@@ -4320,9 +4358,9 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A96" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B96" s="7">
         <v>660</v>
@@ -4356,9 +4394,9 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A97" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B97" s="7">
         <v>503</v>
@@ -4392,9 +4430,9 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A98" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B98" s="7">
         <v>425</v>
@@ -4428,9 +4466,9 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A99" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B99" s="7">
         <v>624</v>
@@ -4469,9 +4507,9 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A100" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B100" s="7">
         <v>503</v>
@@ -4510,9 +4548,9 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A101" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B101" s="7">
         <v>468</v>
@@ -4551,9 +4589,9 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A102" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B102" s="7">
         <v>400</v>
@@ -4592,9 +4630,9 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A103" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B103" s="7">
         <v>284</v>
@@ -4633,9 +4671,9 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A104" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B104" s="7">
         <v>678.65428815072005</v>
@@ -4652,7 +4690,7 @@
       <c r="H104" s="10"/>
       <c r="I104" s="10"/>
       <c r="J104" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K104" s="5"/>
       <c r="L104" s="5"/>
@@ -4668,9 +4706,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A105" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B105" s="7">
         <v>532.018566741325</v>
@@ -4687,7 +4725,7 @@
       <c r="H105" s="10"/>
       <c r="I105" s="10"/>
       <c r="J105" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K105" s="5"/>
       <c r="L105" s="5"/>
@@ -4703,9 +4741,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A106" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B106" s="7">
         <v>498.14385145780801</v>
@@ -4722,7 +4760,7 @@
       <c r="H106" s="10"/>
       <c r="I106" s="10"/>
       <c r="J106" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K106" s="5"/>
       <c r="L106" s="5"/>
@@ -4738,9 +4776,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A107" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B107" s="7">
         <v>443.85150737315701</v>
@@ -4757,7 +4795,7 @@
       <c r="H107" s="10"/>
       <c r="I107" s="10"/>
       <c r="J107" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K107" s="5"/>
       <c r="L107" s="5"/>
@@ -4773,9 +4811,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A108" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B108" s="7">
         <v>305.56845595251298</v>
@@ -4792,7 +4830,7 @@
       <c r="H108" s="10"/>
       <c r="I108" s="10"/>
       <c r="J108" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K108" s="5"/>
       <c r="L108" s="5"/>
@@ -4808,9 +4846,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A109" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B109" s="7">
         <v>265.66124422500502</v>
@@ -4827,7 +4865,7 @@
       <c r="H109" s="10"/>
       <c r="I109" s="10"/>
       <c r="J109" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K109" s="5"/>
       <c r="L109" s="5"/>
@@ -4843,9 +4881,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A110" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B110" s="7">
         <v>190.02320068220101</v>
@@ -4862,7 +4900,7 @@
       <c r="H110" s="10"/>
       <c r="I110" s="10"/>
       <c r="J110" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K110" s="5"/>
       <c r="L110" s="5"/>
@@ -4878,9 +4916,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A111" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B111" s="7">
         <v>181.20649226715901</v>
@@ -4897,7 +4935,7 @@
       <c r="H111" s="10"/>
       <c r="I111" s="10"/>
       <c r="J111" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K111" s="5"/>
       <c r="L111" s="5"/>
@@ -4913,9 +4951,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A112" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B112" s="7">
         <v>20.0925284680287</v>
@@ -4932,7 +4970,7 @@
       <c r="H112" s="10"/>
       <c r="I112" s="10"/>
       <c r="J112" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K112" s="5"/>
       <c r="L112" s="5"/>
@@ -4948,9 +4986,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A113" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B113" s="7">
         <v>20.0925284680287</v>
@@ -4967,7 +5005,7 @@
       <c r="H113" s="10"/>
       <c r="I113" s="10"/>
       <c r="J113" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K113" s="5"/>
       <c r="L113" s="5"/>
@@ -4983,9 +5021,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A114" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B114" s="7">
         <v>350.03304944724903</v>
@@ -5002,7 +5040,7 @@
       <c r="H114" s="10"/>
       <c r="I114" s="10"/>
       <c r="J114" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K114" s="5"/>
       <c r="L114" s="5"/>
@@ -5018,9 +5056,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A115" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B115" s="7">
         <v>449.966953578286</v>
@@ -5037,7 +5075,7 @@
       <c r="H115" s="10"/>
       <c r="I115" s="10"/>
       <c r="J115" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K115" s="5"/>
       <c r="L115" s="5"/>
@@ -5053,9 +5091,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A116" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B116" s="7">
         <v>499.93390564380502</v>
@@ -5072,7 +5110,7 @@
       <c r="H116" s="10"/>
       <c r="I116" s="10"/>
       <c r="J116" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K116" s="5"/>
       <c r="L116" s="5"/>
@@ -5088,9 +5126,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A117" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B117" s="7">
         <v>550.29745107631902</v>
@@ -5107,7 +5145,7 @@
       <c r="H117" s="10"/>
       <c r="I117" s="10"/>
       <c r="J117" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K117" s="5"/>
       <c r="L117" s="5"/>
@@ -5123,9 +5161,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A118" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B118" s="7">
         <v>650.23133402860105</v>
@@ -5142,7 +5180,7 @@
       <c r="H118" s="10"/>
       <c r="I118" s="10"/>
       <c r="J118" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K118" s="5"/>
       <c r="L118" s="5"/>
@@ -5158,9 +5196,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A119" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B119" s="7">
         <v>699.80177744214495</v>
@@ -5177,7 +5215,7 @@
       <c r="H119" s="10"/>
       <c r="I119" s="10"/>
       <c r="J119" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K119" s="5"/>
       <c r="L119" s="5"/>
@@ -5193,9 +5231,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A120" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B120" s="7">
         <v>656.32444121015897</v>
@@ -5212,7 +5250,7 @@
       <c r="H120" s="10"/>
       <c r="I120" s="10"/>
       <c r="J120" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K120" s="5"/>
       <c r="L120" s="5"/>
@@ -5228,9 +5266,9 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A121" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B121" s="7">
         <v>502.66591671410498</v>
@@ -5247,7 +5285,7 @@
       <c r="H121" s="10"/>
       <c r="I121" s="10"/>
       <c r="J121" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K121" s="5"/>
       <c r="L121" s="5"/>
@@ -5263,9 +5301,9 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A122" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B122" s="7">
         <v>453.034597256871</v>
@@ -5282,7 +5320,7 @@
       <c r="H122" s="10"/>
       <c r="I122" s="10"/>
       <c r="J122" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K122" s="5"/>
       <c r="L122" s="5"/>
@@ -5298,9 +5336,9 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A123" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B123" s="7">
         <v>418.88826083605699</v>
@@ -5317,7 +5355,7 @@
       <c r="H123" s="10"/>
       <c r="I123" s="10"/>
       <c r="J123" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K123" s="5"/>
       <c r="L123" s="5"/>
@@ -5333,9 +5371,9 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A124" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B124" s="7">
         <v>349.00737101326899</v>
@@ -5352,7 +5390,7 @@
       <c r="H124" s="10"/>
       <c r="I124" s="10"/>
       <c r="J124" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K124" s="5"/>
       <c r="L124" s="5"/>
@@ -5368,9 +5406,9 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A125" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B125" s="7">
         <v>223.936473865327</v>
@@ -5387,7 +5425,7 @@
       <c r="H125" s="10"/>
       <c r="I125" s="10"/>
       <c r="J125" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K125" s="5"/>
       <c r="L125" s="5"/>
@@ -5403,9 +5441,9 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A126" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B126" s="4">
         <v>157.23199680007701</v>
@@ -5419,7 +5457,7 @@
       <c r="H126" s="5"/>
       <c r="I126" s="5"/>
       <c r="J126" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K126" s="5"/>
       <c r="L126" s="5"/>
@@ -5435,9 +5473,9 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B127" s="4">
         <v>572.943844878596</v>
@@ -5451,7 +5489,7 @@
       <c r="H127" s="5"/>
       <c r="I127" s="5"/>
       <c r="J127" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K127" s="5"/>
       <c r="L127" s="5"/>
@@ -5467,9 +5505,9 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A128" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B128" s="4">
         <v>437.54963542523302</v>
@@ -5483,7 +5521,7 @@
       <c r="H128" s="5"/>
       <c r="I128" s="5"/>
       <c r="J128" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K128" s="5"/>
       <c r="L128" s="5"/>
@@ -5499,9 +5537,9 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B129" s="4">
         <v>373.227449373951</v>
@@ -5515,7 +5553,7 @@
       <c r="H129" s="5"/>
       <c r="I129" s="5"/>
       <c r="J129" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K129" s="5"/>
       <c r="L129" s="5"/>
@@ -5531,9 +5569,9 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B130" s="4">
         <v>331.934210754655</v>
@@ -5547,7 +5585,7 @@
       <c r="H130" s="5"/>
       <c r="I130" s="5"/>
       <c r="J130" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K130" s="5"/>
       <c r="L130" s="5"/>
@@ -5563,9 +5601,9 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B131" s="4">
         <v>313.66987450718301</v>
@@ -5579,7 +5617,7 @@
       <c r="H131" s="5"/>
       <c r="I131" s="5"/>
       <c r="J131" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K131" s="5"/>
       <c r="L131" s="5"/>
@@ -5595,9 +5633,9 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B132" s="4">
         <v>196.93703964299499</v>
@@ -5611,7 +5649,7 @@
       <c r="H132" s="5"/>
       <c r="I132" s="5"/>
       <c r="J132" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K132" s="5"/>
       <c r="L132" s="5"/>
@@ -5627,9 +5665,9 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B133" s="4">
         <v>127.850247708396</v>
@@ -5643,7 +5681,7 @@
       <c r="H133" s="5"/>
       <c r="I133" s="5"/>
       <c r="J133" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K133" s="5"/>
       <c r="L133" s="5"/>
@@ -5659,9 +5697,9 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B134" s="4">
         <v>604.70788763484404</v>
@@ -5675,7 +5713,7 @@
       <c r="H134" s="5"/>
       <c r="I134" s="5"/>
       <c r="J134" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K134" s="5"/>
       <c r="L134" s="5"/>
@@ -5691,9 +5729,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B135" s="4">
         <v>609.47248556636805</v>
@@ -5707,7 +5745,7 @@
       <c r="H135" s="5"/>
       <c r="I135" s="5"/>
       <c r="J135" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K135" s="5"/>
       <c r="L135" s="5"/>
@@ -5723,9 +5761,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B136" s="4">
         <v>424.844026804647</v>
@@ -5739,7 +5777,7 @@
       <c r="H136" s="5"/>
       <c r="I136" s="5"/>
       <c r="J136" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K136" s="5"/>
       <c r="L136" s="5"/>
@@ -5755,9 +5793,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B137" s="4">
         <v>396.65341394285798</v>
@@ -5771,7 +5809,7 @@
       <c r="H137" s="5"/>
       <c r="I137" s="5"/>
       <c r="J137" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K137" s="5"/>
       <c r="L137" s="5"/>
@@ -5787,9 +5825,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A138" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B138" s="4">
         <v>384.34488607354001</v>
@@ -5803,7 +5841,7 @@
       <c r="H138" s="5"/>
       <c r="I138" s="5"/>
       <c r="J138" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K138" s="5"/>
       <c r="L138" s="5"/>
@@ -5819,9 +5857,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A139" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B139" s="4">
         <v>287.46455937782201</v>
@@ -5835,7 +5873,7 @@
       <c r="H139" s="5"/>
       <c r="I139" s="5"/>
       <c r="J139" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K139" s="5"/>
       <c r="L139" s="5"/>
@@ -5851,9 +5889,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A140" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B140" s="4">
         <v>170.334643762366</v>
@@ -5867,7 +5905,7 @@
       <c r="H140" s="5"/>
       <c r="I140" s="5"/>
       <c r="J140" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K140" s="5"/>
       <c r="L140" s="5"/>
@@ -5883,9 +5921,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A141" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B141" s="4">
         <v>481.62222725558098</v>
@@ -5899,7 +5937,7 @@
       <c r="H141" s="5"/>
       <c r="I141" s="5"/>
       <c r="J141" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K141" s="5"/>
       <c r="L141" s="5"/>
@@ -5915,9 +5953,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A142" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B142" s="4">
         <v>485.19569955960401</v>
@@ -5931,7 +5969,7 @@
       <c r="H142" s="5"/>
       <c r="I142" s="5"/>
       <c r="J142" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K142" s="5"/>
       <c r="L142" s="5"/>
@@ -5947,9 +5985,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A143" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B143" s="4">
         <v>337.49291717675999</v>
@@ -5963,7 +6001,7 @@
       <c r="H143" s="5"/>
       <c r="I143" s="5"/>
       <c r="J143" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K143" s="5"/>
       <c r="L143" s="5"/>
@@ -5979,9 +6017,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A144" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B144" s="4">
         <v>325.58138523958002</v>
@@ -5995,7 +6033,7 @@
       <c r="H144" s="5"/>
       <c r="I144" s="5"/>
       <c r="J144" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K144" s="5"/>
       <c r="L144" s="5"/>
@@ -6011,9 +6049,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A145" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B145" s="4">
         <v>293.420304141629</v>
@@ -6027,7 +6065,7 @@
       <c r="H145" s="5"/>
       <c r="I145" s="5"/>
       <c r="J145" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K145" s="5"/>
       <c r="L145" s="5"/>
@@ -6043,9 +6081,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A146" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B146" s="4">
         <v>234.65682716305</v>
@@ -6059,7 +6097,7 @@
       <c r="H146" s="5"/>
       <c r="I146" s="5"/>
       <c r="J146" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K146" s="5"/>
       <c r="L146" s="5"/>
@@ -6075,9 +6113,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A147" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B147" s="4">
         <v>161.20248624102101</v>
@@ -6091,7 +6129,7 @@
       <c r="H147" s="5"/>
       <c r="I147" s="5"/>
       <c r="J147" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K147" s="5"/>
       <c r="L147" s="5"/>
@@ -6107,9 +6145,9 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A148" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B148" s="4">
         <v>123.085639174481</v>
@@ -6123,7 +6161,7 @@
       <c r="H148" s="5"/>
       <c r="I148" s="5"/>
       <c r="J148" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K148" s="5"/>
       <c r="L148" s="5"/>

</xml_diff>